<commit_message>
Increase substitution potential to 20% in 2022 and 50% in 2030
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_IND_Mitigations.xlsx
+++ b/SuppXLS/Scen_B_IND_Mitigations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39AB1C3-35B3-40AD-85F2-7301C7BFC3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CB7291-1E2D-4CEC-B80D-392E7C5608CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5599,9 +5599,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:AG147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T72" sqref="T72"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6254,11 +6252,11 @@
       </c>
       <c r="M12" s="28">
         <f>M7*R12</f>
-        <v>1.26E-4</v>
+        <v>5.04E-4</v>
       </c>
       <c r="N12" s="28">
         <f>N7*S12</f>
-        <v>7.5600000000000005E-4</v>
+        <v>1.2600000000000001E-3</v>
       </c>
       <c r="O12" s="28">
         <f>O7*T12</f>
@@ -6268,10 +6266,10 @@
         <v>5</v>
       </c>
       <c r="R12" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S12" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T12" s="29">
         <v>1</v>
@@ -6336,11 +6334,11 @@
       </c>
       <c r="M13" s="28">
         <f t="shared" ref="M13:O14" si="2">M9*R13</f>
-        <v>2.1960000000000004E-2</v>
+        <v>8.7840000000000015E-2</v>
       </c>
       <c r="N13" s="28">
         <f t="shared" si="2"/>
-        <v>0.13176000000000002</v>
+        <v>0.21960000000000002</v>
       </c>
       <c r="O13" s="28">
         <f t="shared" si="2"/>
@@ -6350,10 +6348,10 @@
         <v>5</v>
       </c>
       <c r="R13" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S13" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T13" s="29">
         <v>1</v>
@@ -6395,11 +6393,11 @@
       </c>
       <c r="M14" s="32">
         <f t="shared" si="2"/>
-        <v>1.0407000000000001E-2</v>
+        <v>4.1628000000000005E-2</v>
       </c>
       <c r="N14" s="32">
         <f t="shared" si="2"/>
-        <v>6.2442000000000004E-2</v>
+        <v>0.10407000000000001</v>
       </c>
       <c r="O14" s="32">
         <f t="shared" si="2"/>
@@ -6409,10 +6407,10 @@
         <v>5</v>
       </c>
       <c r="R14" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S14" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T14" s="29">
         <v>1</v>
@@ -7055,11 +7053,11 @@
       </c>
       <c r="M24" s="28">
         <f>M22*R24</f>
-        <v>3.1341000000000001E-2</v>
+        <v>0.125364</v>
       </c>
       <c r="N24" s="28">
         <f>N22*S24</f>
-        <v>0.18804599999999996</v>
+        <v>0.31340999999999997</v>
       </c>
       <c r="O24" s="28">
         <f>O22*T24</f>
@@ -7069,10 +7067,10 @@
         <v>5</v>
       </c>
       <c r="R24" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S24" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T24" s="29">
         <v>1</v>
@@ -7153,11 +7151,11 @@
       </c>
       <c r="M26" s="28">
         <f>M18*R26</f>
-        <v>1.6700000000000002E-4</v>
+        <v>6.6800000000000008E-4</v>
       </c>
       <c r="N26" s="28">
         <f>N18*S26</f>
-        <v>1.0020000000000001E-3</v>
+        <v>1.67E-3</v>
       </c>
       <c r="O26" s="28">
         <f>O18*T26</f>
@@ -7167,10 +7165,10 @@
         <v>5</v>
       </c>
       <c r="R26" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S26" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T26" s="29">
         <v>1</v>
@@ -7212,11 +7210,11 @@
       </c>
       <c r="M27" s="32">
         <f>M21*R27</f>
-        <v>1.1575000000000001E-3</v>
+        <v>4.6300000000000004E-3</v>
       </c>
       <c r="N27" s="32">
         <f>N21*S27</f>
-        <v>6.9449999999999998E-3</v>
+        <v>1.1575E-2</v>
       </c>
       <c r="O27" s="32">
         <f>O21*T27</f>
@@ -7226,10 +7224,10 @@
         <v>5</v>
       </c>
       <c r="R27" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S27" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T27" s="29">
         <v>1</v>
@@ -7713,11 +7711,11 @@
       </c>
       <c r="M34" s="28">
         <f>M29*R34</f>
-        <v>2.7500000000000004E-5</v>
+        <v>1.1000000000000002E-4</v>
       </c>
       <c r="N34" s="28">
         <f>N29*S34</f>
-        <v>1.65E-4</v>
+        <v>2.7500000000000002E-4</v>
       </c>
       <c r="O34" s="28">
         <f>O29*T34</f>
@@ -7727,10 +7725,10 @@
         <v>5</v>
       </c>
       <c r="R34" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S34" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T34" s="29">
         <v>1</v>
@@ -7798,11 +7796,11 @@
       </c>
       <c r="M35" s="28">
         <f t="shared" ref="M35:O36" si="7">M31*R35</f>
-        <v>1.0090000000000001E-3</v>
+        <v>4.0360000000000005E-3</v>
       </c>
       <c r="N35" s="28">
         <f t="shared" si="7"/>
-        <v>6.0539999999999995E-3</v>
+        <v>1.009E-2</v>
       </c>
       <c r="O35" s="28">
         <f t="shared" si="7"/>
@@ -7812,10 +7810,10 @@
         <v>5</v>
       </c>
       <c r="R35" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S35" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T35" s="29">
         <v>1</v>
@@ -7857,11 +7855,11 @@
       </c>
       <c r="M36" s="32">
         <f t="shared" si="7"/>
-        <v>3.4575999999999996E-2</v>
+        <v>0.13830399999999998</v>
       </c>
       <c r="N36" s="32">
         <f t="shared" si="7"/>
-        <v>0.20745599999999997</v>
+        <v>0.34575999999999996</v>
       </c>
       <c r="O36" s="32">
         <f t="shared" si="7"/>
@@ -7871,10 +7869,10 @@
         <v>5</v>
       </c>
       <c r="R36" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S36" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T36" s="29">
         <v>1</v>
@@ -8425,11 +8423,11 @@
       </c>
       <c r="M44" s="28">
         <f>M38*R44</f>
-        <v>3.3500000000000001E-5</v>
+        <v>1.34E-4</v>
       </c>
       <c r="N44" s="28">
         <f>N38*S44</f>
-        <v>2.0100000000000001E-4</v>
+        <v>3.3500000000000001E-4</v>
       </c>
       <c r="O44" s="28">
         <f>O38*T44</f>
@@ -8439,10 +8437,10 @@
         <v>5</v>
       </c>
       <c r="R44" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S44" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T44" s="29">
         <v>1</v>
@@ -8484,11 +8482,11 @@
       </c>
       <c r="M45" s="28">
         <f t="shared" ref="M45:O46" si="17">M40*R45</f>
-        <v>6.0599999999999998E-4</v>
+        <v>2.4239999999999999E-3</v>
       </c>
       <c r="N45" s="28">
         <f t="shared" si="17"/>
-        <v>3.6359999999999995E-3</v>
+        <v>6.0599999999999994E-3</v>
       </c>
       <c r="O45" s="28">
         <f t="shared" si="17"/>
@@ -8498,10 +8496,10 @@
         <v>5</v>
       </c>
       <c r="R45" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S45" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T45" s="29">
         <v>1</v>
@@ -8537,11 +8535,11 @@
       </c>
       <c r="M46" s="32">
         <f t="shared" si="17"/>
-        <v>2.8720000000000004E-3</v>
+        <v>1.1488000000000002E-2</v>
       </c>
       <c r="N46" s="32">
         <f t="shared" si="17"/>
-        <v>1.7232000000000001E-2</v>
+        <v>2.8720000000000002E-2</v>
       </c>
       <c r="O46" s="32">
         <f t="shared" si="17"/>
@@ -8551,10 +8549,10 @@
         <v>5</v>
       </c>
       <c r="R46" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S46" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T46" s="29">
         <v>1</v>
@@ -9044,11 +9042,11 @@
       </c>
       <c r="M53" s="28">
         <f>M48*R53</f>
-        <v>1.295E-4</v>
+        <v>5.1800000000000001E-4</v>
       </c>
       <c r="N53" s="28">
         <f>N48*S53</f>
-        <v>7.7699999999999991E-4</v>
+        <v>1.2949999999999999E-3</v>
       </c>
       <c r="O53" s="28">
         <f>O48*T53</f>
@@ -9058,10 +9056,10 @@
         <v>5</v>
       </c>
       <c r="R53" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S53" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T53" s="29">
         <v>1</v>
@@ -9123,11 +9121,11 @@
       </c>
       <c r="M54" s="28">
         <f t="shared" ref="M54:O55" si="26">M50*R54</f>
-        <v>1.0659999999999999E-3</v>
+        <v>4.2639999999999996E-3</v>
       </c>
       <c r="N54" s="28">
         <f t="shared" si="26"/>
-        <v>6.3959999999999998E-3</v>
+        <v>1.0659999999999999E-2</v>
       </c>
       <c r="O54" s="28">
         <f t="shared" si="26"/>
@@ -9137,10 +9135,10 @@
         <v>5</v>
       </c>
       <c r="R54" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S54" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T54" s="29">
         <v>1</v>
@@ -9182,11 +9180,11 @@
       </c>
       <c r="M55" s="32">
         <f t="shared" si="26"/>
-        <v>2.4456500000000003E-2</v>
+        <v>9.782600000000001E-2</v>
       </c>
       <c r="N55" s="32">
         <f t="shared" si="26"/>
-        <v>0.14673900000000001</v>
+        <v>0.244565</v>
       </c>
       <c r="O55" s="32">
         <f t="shared" si="26"/>
@@ -9196,10 +9194,10 @@
         <v>5</v>
       </c>
       <c r="R55" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S55" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T55" s="29">
         <v>1</v>
@@ -9763,11 +9761,11 @@
       </c>
       <c r="M64" s="28">
         <f>M57*R64</f>
-        <v>7.400000000000001E-5</v>
+        <v>2.9600000000000004E-4</v>
       </c>
       <c r="N64" s="28">
         <f>N57*S64</f>
-        <v>4.4399999999999995E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="O64" s="28">
         <f>O57*T64</f>
@@ -9777,10 +9775,10 @@
         <v>5</v>
       </c>
       <c r="R64" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S64" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T64" s="29">
         <v>1</v>
@@ -9810,11 +9808,11 @@
       </c>
       <c r="M65" s="28">
         <f>M60*R65</f>
-        <v>9.1349999999999992E-4</v>
+        <v>3.6539999999999997E-3</v>
       </c>
       <c r="N65" s="28">
         <f>N60*S65</f>
-        <v>5.4809999999999989E-3</v>
+        <v>9.134999999999999E-3</v>
       </c>
       <c r="O65" s="28">
         <f>O60*T65</f>
@@ -9824,10 +9822,10 @@
         <v>5</v>
       </c>
       <c r="R65" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S65" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T65" s="29">
         <v>1</v>
@@ -9857,11 +9855,11 @@
       </c>
       <c r="M66" s="32">
         <f>M62*R66</f>
-        <v>2.8210499999999999E-2</v>
+        <v>0.112842</v>
       </c>
       <c r="N66" s="32">
         <f>N62*S66</f>
-        <v>0.169263</v>
+        <v>0.28210499999999999</v>
       </c>
       <c r="O66" s="32">
         <f>O62*T66</f>
@@ -9871,10 +9869,10 @@
         <v>5</v>
       </c>
       <c r="R66" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S66" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T66" s="29">
         <v>1</v>
@@ -10286,11 +10284,11 @@
       </c>
       <c r="M73" s="28">
         <f>M68*R73</f>
-        <v>9.4550000000000005E-4</v>
+        <v>3.7820000000000002E-3</v>
       </c>
       <c r="N73" s="28">
         <f>N68*S73</f>
-        <v>5.6730000000000001E-3</v>
+        <v>9.4549999999999999E-3</v>
       </c>
       <c r="O73" s="28">
         <f>O68*T73</f>
@@ -10300,10 +10298,10 @@
         <v>5</v>
       </c>
       <c r="R73" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S73" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T73" s="29">
         <v>1</v>
@@ -10359,11 +10357,11 @@
       </c>
       <c r="M74" s="28">
         <f t="shared" ref="M74:O75" si="46">M70*R74</f>
-        <v>1.1845E-3</v>
+        <v>4.738E-3</v>
       </c>
       <c r="N74" s="28">
         <f t="shared" si="46"/>
-        <v>7.1069999999999996E-3</v>
+        <v>1.1845E-2</v>
       </c>
       <c r="O74" s="28">
         <f t="shared" si="46"/>
@@ -10373,10 +10371,10 @@
         <v>5</v>
       </c>
       <c r="R74" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S74" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T74" s="29">
         <v>1</v>
@@ -10406,11 +10404,11 @@
       </c>
       <c r="M75" s="32">
         <f t="shared" si="46"/>
-        <v>1.6687000000000004E-2</v>
+        <v>6.6748000000000016E-2</v>
       </c>
       <c r="N75" s="32">
         <f t="shared" si="46"/>
-        <v>0.100122</v>
+        <v>0.16687000000000002</v>
       </c>
       <c r="O75" s="32">
         <f t="shared" si="46"/>
@@ -10420,10 +10418,10 @@
         <v>5</v>
       </c>
       <c r="R75" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S75" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T75" s="29">
         <v>1</v>
@@ -10978,11 +10976,11 @@
       </c>
       <c r="M84" s="24">
         <f>(M77+M81)*R84+$L84</f>
-        <v>2.6452800000000005E-2</v>
+        <v>8.8051199999999996E-2</v>
       </c>
       <c r="N84" s="24">
         <f t="shared" ref="N84:O84" si="59">(N77+N81)*S84+$L84</f>
-        <v>0.1291168</v>
+        <v>0.21124800000000002</v>
       </c>
       <c r="O84" s="24">
         <f t="shared" si="59"/>
@@ -10992,12 +10990,11 @@
         <v>5</v>
       </c>
       <c r="R84" s="29">
-        <f>5%*80%</f>
-        <v>4.0000000000000008E-2</v>
+        <v>0.16</v>
       </c>
       <c r="S84" s="29">
-        <f>30%*80%</f>
-        <v>0.24</v>
+        <f>50%*80%</f>
+        <v>0.4</v>
       </c>
       <c r="T84" s="29">
         <f>100%*80%</f>
@@ -11118,11 +11115,11 @@
       </c>
       <c r="M87" s="28">
         <f>M78*R87</f>
-        <v>1.1200000000000001E-4</v>
+        <v>4.4800000000000005E-4</v>
       </c>
       <c r="N87" s="28">
         <f>N78*S87</f>
-        <v>6.7200000000000007E-4</v>
+        <v>1.1200000000000001E-3</v>
       </c>
       <c r="O87" s="28">
         <f>O78*T87</f>
@@ -11132,10 +11129,10 @@
         <v>5</v>
       </c>
       <c r="R87" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S87" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T87" s="29">
         <v>1</v>
@@ -11165,11 +11162,11 @@
       </c>
       <c r="M88" s="28">
         <f>M80*R88</f>
-        <v>1.4255000000000001E-3</v>
+        <v>5.7020000000000005E-3</v>
       </c>
       <c r="N88" s="28">
         <f>N80*S88</f>
-        <v>8.5529999999999998E-3</v>
+        <v>1.4255E-2</v>
       </c>
       <c r="O88" s="28">
         <f>O80*T88</f>
@@ -11179,10 +11176,10 @@
         <v>5</v>
       </c>
       <c r="R88" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S88" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T88" s="29">
         <v>1</v>
@@ -11212,11 +11209,11 @@
       </c>
       <c r="M89" s="28">
         <f>M82*R89</f>
-        <v>3.823E-3</v>
+        <v>1.5292E-2</v>
       </c>
       <c r="N89" s="28">
         <f>N82*S89</f>
-        <v>2.2938E-2</v>
+        <v>3.823E-2</v>
       </c>
       <c r="O89" s="28">
         <f>O82*T89</f>
@@ -11226,10 +11223,10 @@
         <v>5</v>
       </c>
       <c r="R89" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S89" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T89" s="29">
         <v>1</v>
@@ -11263,7 +11260,7 @@
       </c>
       <c r="N90" s="32">
         <f>(N77+N81)*S90</f>
-        <v>3.0799199999999999E-2</v>
+        <v>5.1332000000000003E-2</v>
       </c>
       <c r="O90" s="32">
         <f>(O77+O81)*T90</f>
@@ -11277,8 +11274,8 @@
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="S90" s="29">
-        <f>30%*20%</f>
-        <v>0.06</v>
+        <f>50%*20%</f>
+        <v>0.1</v>
       </c>
       <c r="T90" s="29">
         <f>100%*20%</f>
@@ -11696,10 +11693,10 @@
         <v>5</v>
       </c>
       <c r="R97" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S97" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T97" s="29">
         <v>1</v>
@@ -11760,10 +11757,10 @@
         <v>5</v>
       </c>
       <c r="R98" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S98" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T98" s="29">
         <v>1</v>
@@ -11793,11 +11790,11 @@
       </c>
       <c r="M99" s="28">
         <f>M93*R97</f>
-        <v>4.5000000000000003E-5</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="N99" s="28">
         <f>N93*S97</f>
-        <v>2.7E-4</v>
+        <v>4.4999999999999999E-4</v>
       </c>
       <c r="O99" s="28">
         <f>O93*T97</f>
@@ -11807,10 +11804,10 @@
         <v>5</v>
       </c>
       <c r="R99" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S99" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T99" s="29">
         <v>1</v>
@@ -11840,11 +11837,11 @@
       </c>
       <c r="M100" s="28">
         <f t="shared" ref="M100:O101" si="72">M96*R98</f>
-        <v>1.7900000000000001E-4</v>
+        <v>7.1600000000000006E-4</v>
       </c>
       <c r="N100" s="28">
         <f t="shared" si="72"/>
-        <v>1.0739999999999999E-3</v>
+        <v>1.7899999999999999E-3</v>
       </c>
       <c r="O100" s="28">
         <f t="shared" si="72"/>
@@ -11878,11 +11875,11 @@
       </c>
       <c r="M101" s="32">
         <f t="shared" si="72"/>
-        <v>4.3324000000000001E-2</v>
+        <v>0.17329600000000001</v>
       </c>
       <c r="N101" s="32">
         <f t="shared" si="72"/>
-        <v>0.25994399999999995</v>
+        <v>0.43323999999999996</v>
       </c>
       <c r="O101" s="32">
         <f t="shared" si="72"/>
@@ -12177,10 +12174,10 @@
         <v>5</v>
       </c>
       <c r="R106" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S106" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T106" s="29">
         <v>1</v>
@@ -12242,10 +12239,10 @@
         <v>5</v>
       </c>
       <c r="R107" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S107" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T107" s="29">
         <v>1</v>
@@ -12316,11 +12313,11 @@
       </c>
       <c r="M108" s="28">
         <f>M103*R106</f>
-        <v>4.2650000000000001E-4</v>
+        <v>1.7060000000000001E-3</v>
       </c>
       <c r="N108" s="28">
         <f>N103*S106</f>
-        <v>2.5589999999999996E-3</v>
+        <v>4.2649999999999997E-3</v>
       </c>
       <c r="O108" s="28">
         <f>O103*T106</f>
@@ -12330,10 +12327,10 @@
         <v>5</v>
       </c>
       <c r="R108" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S108" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T108" s="29">
         <v>1</v>
@@ -12389,11 +12386,11 @@
       </c>
       <c r="M109" s="28">
         <f t="shared" ref="M109:O110" si="84">M105*R107</f>
-        <v>1.8610000000000002E-3</v>
+        <v>7.444000000000001E-3</v>
       </c>
       <c r="N109" s="28">
         <f t="shared" si="84"/>
-        <v>1.1166000000000001E-2</v>
+        <v>1.8610000000000002E-2</v>
       </c>
       <c r="O109" s="28">
         <f t="shared" si="84"/>
@@ -12427,11 +12424,11 @@
       </c>
       <c r="M110" s="32">
         <f t="shared" si="84"/>
-        <v>2.1146000000000002E-2</v>
+        <v>8.4584000000000006E-2</v>
       </c>
       <c r="N110" s="32">
         <f t="shared" si="84"/>
-        <v>0.12687599999999999</v>
+        <v>0.21146000000000001</v>
       </c>
       <c r="O110" s="32">
         <f t="shared" si="84"/>
@@ -12726,10 +12723,10 @@
         <v>5</v>
       </c>
       <c r="R115" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S115" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T115" s="29">
         <v>1</v>
@@ -12791,10 +12788,10 @@
         <v>5</v>
       </c>
       <c r="R116" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S116" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T116" s="29">
         <v>1</v>
@@ -12865,11 +12862,11 @@
       </c>
       <c r="M117" s="28">
         <f>M112*R115</f>
-        <v>1.145E-4</v>
+        <v>4.5800000000000002E-4</v>
       </c>
       <c r="N117" s="28">
         <f>N112*S115</f>
-        <v>6.87E-4</v>
+        <v>1.145E-3</v>
       </c>
       <c r="O117" s="28">
         <f>O112*T115</f>
@@ -12879,10 +12876,10 @@
         <v>5</v>
       </c>
       <c r="R117" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S117" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T117" s="29">
         <v>1</v>
@@ -12938,11 +12935,11 @@
       </c>
       <c r="M118" s="28">
         <f t="shared" ref="M118:O119" si="96">M114*R116</f>
-        <v>2.1999999999999998E-4</v>
+        <v>8.7999999999999992E-4</v>
       </c>
       <c r="N118" s="28">
         <f t="shared" si="96"/>
-        <v>1.3199999999999998E-3</v>
+        <v>2.1999999999999997E-3</v>
       </c>
       <c r="O118" s="28">
         <f t="shared" si="96"/>
@@ -12976,11 +12973,11 @@
       </c>
       <c r="M119" s="32">
         <f t="shared" si="96"/>
-        <v>8.8735000000000012E-3</v>
+        <v>3.5494000000000005E-2</v>
       </c>
       <c r="N119" s="32">
         <f t="shared" si="96"/>
-        <v>5.3241000000000004E-2</v>
+        <v>8.8735000000000008E-2</v>
       </c>
       <c r="O119" s="32">
         <f t="shared" si="96"/>
@@ -13275,10 +13272,10 @@
         <v>5</v>
       </c>
       <c r="R124" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S124" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T124" s="29">
         <v>1</v>
@@ -13340,10 +13337,10 @@
         <v>5</v>
       </c>
       <c r="R125" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S125" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T125" s="29">
         <v>1</v>
@@ -13414,11 +13411,11 @@
       </c>
       <c r="M126" s="28">
         <f>M121*R124</f>
-        <v>6.7000000000000002E-4</v>
+        <v>2.6800000000000001E-3</v>
       </c>
       <c r="N126" s="28">
         <f>N121*S124</f>
-        <v>4.0200000000000001E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="O126" s="28">
         <f>O121*T124</f>
@@ -13428,10 +13425,10 @@
         <v>5</v>
       </c>
       <c r="R126" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S126" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T126" s="29">
         <v>1</v>
@@ -13487,11 +13484,11 @@
       </c>
       <c r="M127" s="28">
         <f t="shared" ref="M127:O128" si="108">M123*R126</f>
-        <v>2.2825000000000002E-3</v>
+        <v>9.130000000000001E-3</v>
       </c>
       <c r="N127" s="28">
         <f t="shared" si="108"/>
-        <v>1.3695000000000001E-2</v>
+        <v>2.2825000000000002E-2</v>
       </c>
       <c r="O127" s="28">
         <f t="shared" si="108"/>
@@ -13880,10 +13877,10 @@
         <v>5</v>
       </c>
       <c r="R134" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S134" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T134" s="29">
         <v>1</v>
@@ -13959,10 +13956,10 @@
         <v>5</v>
       </c>
       <c r="R135" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S135" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T135" s="29">
         <v>1</v>
@@ -14018,11 +14015,11 @@
       </c>
       <c r="M136" s="28">
         <f>M130*R134</f>
-        <v>1.8800000000000002E-4</v>
+        <v>7.5200000000000006E-4</v>
       </c>
       <c r="N136" s="28">
         <f>N130*S134</f>
-        <v>1.1279999999999999E-3</v>
+        <v>1.8799999999999999E-3</v>
       </c>
       <c r="O136" s="28">
         <f>O130*T134</f>
@@ -14032,10 +14029,10 @@
         <v>5</v>
       </c>
       <c r="R136" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S136" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T136" s="29">
         <v>1</v>
@@ -14065,11 +14062,11 @@
       </c>
       <c r="M137" s="28">
         <f t="shared" ref="M137:O138" si="120">M133*R135</f>
-        <v>8.5399999999999994E-4</v>
+        <v>3.4159999999999998E-3</v>
       </c>
       <c r="N137" s="28">
         <f t="shared" si="120"/>
-        <v>5.1239999999999992E-3</v>
+        <v>8.539999999999999E-3</v>
       </c>
       <c r="O137" s="28">
         <f t="shared" si="120"/>
@@ -14103,11 +14100,11 @@
       </c>
       <c r="M138" s="32">
         <f t="shared" si="120"/>
-        <v>2.1451000000000001E-2</v>
+        <v>8.5804000000000005E-2</v>
       </c>
       <c r="N138" s="32">
         <f t="shared" si="120"/>
-        <v>0.12870599999999999</v>
+        <v>0.21451000000000001</v>
       </c>
       <c r="O138" s="32">
         <f t="shared" si="120"/>
@@ -14402,10 +14399,10 @@
         <v>5</v>
       </c>
       <c r="R143" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S143" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T143" s="29">
         <v>1</v>
@@ -14467,10 +14464,10 @@
         <v>5</v>
       </c>
       <c r="R144" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S144" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T144" s="29">
         <v>1</v>
@@ -14541,11 +14538,11 @@
       </c>
       <c r="M145" s="28">
         <f>M140*R143</f>
-        <v>8.0249999999999994E-4</v>
+        <v>3.2099999999999997E-3</v>
       </c>
       <c r="N145" s="28">
         <f>N140*S143</f>
-        <v>4.814999999999999E-3</v>
+        <v>8.0249999999999991E-3</v>
       </c>
       <c r="O145" s="28">
         <f>O140*T143</f>
@@ -14555,10 +14552,10 @@
         <v>5</v>
       </c>
       <c r="R145" s="29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="S145" s="29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T145" s="29">
         <v>1</v>
@@ -14614,11 +14611,11 @@
       </c>
       <c r="M146" s="28">
         <f t="shared" ref="M146:O147" si="132">M142*R144</f>
-        <v>3.5243999999999998E-2</v>
+        <v>0.14097599999999999</v>
       </c>
       <c r="N146" s="28">
         <f t="shared" si="132"/>
-        <v>0.21146399999999999</v>
+        <v>0.35243999999999998</v>
       </c>
       <c r="O146" s="28">
         <f t="shared" si="132"/>
@@ -14649,11 +14646,11 @@
       </c>
       <c r="M147" s="32">
         <f t="shared" si="132"/>
-        <v>3.6245000000000001E-3</v>
+        <v>1.4498E-2</v>
       </c>
       <c r="N147" s="32">
         <f t="shared" si="132"/>
-        <v>2.1746999999999999E-2</v>
+        <v>3.6244999999999999E-2</v>
       </c>
       <c r="O147" s="32">
         <f t="shared" si="132"/>

</xml_diff>